<commit_message>
PROS-8878 - CCRU - Add additional level of results for Top Gaps KPIs - fix
</commit_message>
<xml_diff>
--- a/Projects/CCRU_SAND/Data/KPIs_2019/PoS 2019 - IC Canteen - EDU.xlsx
+++ b/Projects/CCRU_SAND/Data/KPIs_2019/PoS 2019 - IC Canteen - EDU.xlsx
@@ -15,6 +15,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0" vbProcedure="false">Canteen!$A$1:$AL$54</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Canteen!$A$1:$AL$54</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Canteen!$A$1:$AL$54</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Canteen!$A$1:$AL$54</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -219,7 +220,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Coca-Cola - 0.25L Slim/Coca-Cola - 0.33L Glass</t>
+    <t xml:space="preserve">Coca-Cola - 0.25L Slim/0.33L Glass</t>
   </si>
   <si>
     <t xml:space="preserve">Кока-Кола - 0.25л слим/Кока-Кола - 0.33л стекло</t>
@@ -249,7 +250,7 @@
     <t xml:space="preserve">BINARY</t>
   </si>
   <si>
-    <t xml:space="preserve">Coca-Cola Zero/Cherry - 0.25L /Coca-Cola Zero - 0.33L Glass</t>
+    <t xml:space="preserve">Coca-Cola Zero - 0.25L Slim/0.33L Glass/Coca-Cola Zero Cherry - 0.25L Slim</t>
   </si>
   <si>
     <t xml:space="preserve">Кока-Кола Зеро/Вишня - 0.25л слим/Кока-Кола Зеро - 0.33л стекло</t>
@@ -297,7 +298,7 @@
     <t xml:space="preserve">Спрайт - 0.5л</t>
   </si>
   <si>
-    <t xml:space="preserve">Coca-Cola Zero/Zero Cherry - 0.5L</t>
+    <t xml:space="preserve">Coca-Cola Zero/Coca-Cola Zero Cherry - 0.5L</t>
   </si>
   <si>
     <t xml:space="preserve">Кока-Кола Зеро/Вишня - 0.5л</t>
@@ -315,7 +316,7 @@
     <t xml:space="preserve">Фанта Апельсин - 0.5л</t>
   </si>
   <si>
-    <t xml:space="preserve">Fanta Citrus/Pear - 0.5L - 0.5L</t>
+    <t xml:space="preserve">Fanta Citrus - 0.5L/Fanta Pear - 0.5L</t>
   </si>
   <si>
     <t xml:space="preserve">Фанта Цитрус/Груша - 0.5л - 0.5л</t>
@@ -357,7 +358,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">BonAqua Still/Carb 0-33/0.5L SmartWater Still-0.6L</t>
+    <t xml:space="preserve">BonAqua Still/Carb - 0.5L/0.33L Glass/SmartWater Still - 0.6L</t>
   </si>
   <si>
     <t xml:space="preserve">БонАква Негаз/Газ-0.5л /Смарт вода-0.6л/БонАква Негаз/ Газ-0.33л стекло</t>
@@ -421,7 +422,7 @@
     <t xml:space="preserve">4607042430879, 5449000027450</t>
   </si>
   <si>
-    <t xml:space="preserve">Fuze Berry-Hibiscus/Lemon-Lemongrass - 0.5L</t>
+    <t xml:space="preserve">Fuze Berry-Hibiscus - 0.5L/Fuze Lemon-Lemongrass - 0.5L</t>
   </si>
   <si>
     <t xml:space="preserve">Фьюз Лесн.ягоды/Лимон - 0.5л</t>
@@ -433,7 +434,7 @@
     <t xml:space="preserve">5449000259455, 5449000235947, 5449000193124, 5449000189301</t>
   </si>
   <si>
-    <t xml:space="preserve">Fuze Green Strawberry-Raspberry/Peach-Rose/Green Citrus - 0.5L</t>
+    <t xml:space="preserve">Fuze Green Strawberry-Raspberry - 0.5L/Peach-Rose/Green Citrus - 0.5L</t>
   </si>
   <si>
     <t xml:space="preserve">Фьюз Зеленый Клубника/Персик/Зеленый Цитрус - 0.5л</t>
@@ -461,7 +462,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Dobriy - Apple -0.33L/Rich - Apple - 0.3L/0.2L Glass</t>
+    <t xml:space="preserve">Dobriy - Apple - 0.33L/Rich - Apple - 0.3L/0.2L Glass</t>
   </si>
   <si>
     <t xml:space="preserve">Добрый - Яблоко - 0.33л/Рич - Яблоко - 0.3л/0.2л стекло</t>
@@ -485,7 +486,7 @@
     <t xml:space="preserve">Палпи - Манго Ананас - 0.45л</t>
   </si>
   <si>
-    <t xml:space="preserve">Dobriy - Multifruit - 0.33L/ Rich - Orange - 0.2L Glass/0.3L </t>
+    <t xml:space="preserve">Dobriy - Multifruit - 0.33L/Rich - Orange - 0.2L Glass/0.3L </t>
   </si>
   <si>
     <t xml:space="preserve">Добрый-Мультифрут-0.33л/ Рич- Апельсин-0.2л стекло/ 0.3л </t>
@@ -497,7 +498,7 @@
     <t xml:space="preserve">4607174579286, 4650075420362, 4650075421024</t>
   </si>
   <si>
-    <t xml:space="preserve">Dobriy-Tomato-0.33L /Rich-Cherry-0.2L Glass/0.3L </t>
+    <t xml:space="preserve">Dobriy - Tomato - 0.33L/Rich - Cherry - 0.2L Glass/0.3L </t>
   </si>
   <si>
     <t xml:space="preserve">Добрый-Томат-0.33л/ Рич-Вишня-0.2л стекло/0.3л </t>
@@ -518,7 +519,7 @@
     <t xml:space="preserve">Pulpy - Tropical - 0.45L, Pulpy - Guava - 0.45L, Pulpy - Watermelon Strawberry - 0.45L</t>
   </si>
   <si>
-    <t xml:space="preserve">Dobriy-Peach-Apple/Orange-0.33L/Rich-Peach/Pineapple/Grapefruit/Tomato-0.2L Glass</t>
+    <t xml:space="preserve">Dobriy - Peach-Apple/Orange - 0.33L/Rich - Peach/Pineapple/Grapefruit/Tomato - 0.2L Glass</t>
   </si>
   <si>
     <t xml:space="preserve">Добрый-Персик/Апельсин-0.33л /Рич-Персик/Ананас/Грейпфру/Томат-0.2л стекло</t>
@@ -1208,47 +1209,47 @@
   </sheetPr>
   <dimension ref="1:56"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="N38" activeCellId="0" sqref="N38"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="F1" activeCellId="0" sqref="F:F"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.1781376518219"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="2" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="2" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="2" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="14.6761133603239"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="69.3076923076923"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="71.4493927125506"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="41.0283400809717"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="69.9473684210526"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="72.0890688259109"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="41.3481781376518"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="16.1740890688259"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="2" width="9"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="2" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="72.9271255060729"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="81.7327935222672"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="45.6315789473684"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="2" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="2" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="2" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="73.4817813765182"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="82.4817813765182"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="46.0607287449393"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="2" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="2" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="2" width="12.4251012145749"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="2" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="17.246963562753"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="21.9595141700405"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="22.3886639676113"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="2" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="24.8502024291498"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="2" width="25.3886639676113"/>
-    <col collapsed="false" hidden="false" max="29" min="28" style="2" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="2" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="2" width="12.3198380566802"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="2" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="2" width="59.4493927125506"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="2" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="2" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="2" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="25.0647773279352"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="2" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="29" min="28" style="2" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="2" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="2" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="2" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="2" width="59.9878542510121"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="2" width="21.5303643724696"/>
     <col collapsed="false" hidden="false" max="35" min="35" style="2" width="7.60728744939271"/>
     <col collapsed="false" hidden="false" max="36" min="36" style="2" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="37" min="37" style="2" width="10.6032388663968"/>
@@ -58606,7 +58607,7 @@
       <c r="AMI54" s="0"/>
       <c r="AMJ54" s="0"/>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="8" t="n">
         <v>51</v>
       </c>
@@ -59658,7 +59659,7 @@
       <c r="AMI55" s="0"/>
       <c r="AMJ55" s="0"/>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="8" t="n">
         <v>401</v>
       </c>

</xml_diff>